<commit_message>
Added code to remove unnecessary columns and created final dataframe to be used downstream
</commit_message>
<xml_diff>
--- a/notes/fields.xlsx
+++ b/notes/fields.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\philadelphia_housing_analysis\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6158D148-E2A8-4BC0-957B-380860879BDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28080B48-7555-4603-82A0-87E8C8AA1692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
+    <sheet name="fields to keep" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$1:$D$73</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="205">
   <si>
     <t>Field Name</t>
   </si>
@@ -643,7 +655,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1127,10 +1139,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1494,10 +1507,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1520,7 +1536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1542,7 +1558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1553,7 +1569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1575,7 +1591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1619,7 +1635,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1630,7 +1646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1734,7 +1750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1753,7 +1769,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
@@ -1764,7 +1780,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
@@ -1797,7 +1813,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>78</v>
       </c>
@@ -1811,7 +1827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
@@ -1825,7 +1841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>84</v>
       </c>
@@ -1839,7 +1855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
@@ -1853,7 +1869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
@@ -1867,7 +1883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
@@ -1944,7 +1960,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>113</v>
       </c>
@@ -1952,7 +1968,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
@@ -1963,7 +1979,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>118</v>
       </c>
@@ -1974,7 +1990,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>121</v>
       </c>
@@ -1985,7 +2001,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>124</v>
       </c>
@@ -2007,7 +2023,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>130</v>
       </c>
@@ -2018,7 +2034,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>133</v>
       </c>
@@ -2051,7 +2067,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>142</v>
       </c>
@@ -2062,7 +2078,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>145</v>
       </c>
@@ -2081,7 +2097,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>150</v>
       </c>
@@ -2089,7 +2105,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>152</v>
       </c>
@@ -2097,7 +2113,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>154</v>
       </c>
@@ -2141,7 +2157,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>163</v>
       </c>
@@ -2212,7 +2228,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>182</v>
       </c>
@@ -2234,7 +2250,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>188</v>
       </c>
@@ -2298,8 +2314,406 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D73"/>
+  <autoFilter ref="A1:D73" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425ECA68-E9BA-4D0B-88FA-29D54F3D053D}">
+  <dimension ref="A1:D42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D42" sqref="D1:D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="D1" t="str">
+        <f>"['"&amp;A1&amp;"',"</f>
+        <v>['basements',</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"'"&amp;A2&amp;"',"</f>
+        <v>'building_code_description',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D42" si="0">"'"&amp;A3&amp;"',"</f>
+        <v>'category_code_description',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>'census_tract',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>'central_air',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>'depth',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>'exempt_building',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>'exempt_land',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>'exterior_condition',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>'fireplaces',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>'frontage',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>'fuel',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>'garage_spaces',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>'garage_type',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>'geographic_ward',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>'interior_condition',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>'location',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>'market_value',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>'market_value_date',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>'number_of_bathrooms',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>'number_of_bedrooms',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>'number_of_rooms',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>'number_stories',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>'quality_grade',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>'sale_date',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>'sale_price',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>'shape',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>'street_designation',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>159</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>'street_direction',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>'street_name',</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>'taxable_building',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>'taxable_land',</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>'topography',</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>'total_area',</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>177</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>'total_livable_area',</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>'type_heater',</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>'unit',</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>'view',</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>193</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>'year_built',</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>196</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>'year_built_estimate',</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>'zip_code',</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" t="str">
+        <f>"'"&amp;A42&amp;"']"</f>
+        <v>'zoning']</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>